<commit_message>
to load the Data item to the queue
</commit_message>
<xml_diff>
--- a/Data/Config.xlsx
+++ b/Data/Config.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\UIPath Full Projects\REF_CSH_Dispatcher\Data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Projects\GenerateYearly Report for Vendor\REF_GYR_Dispatcher\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7EE189AE-7E2B-4C2A-BC0A-60FC6C5882A1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{44A98E8F-1810-4A94-821A-F0DB64315019}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3100" yWindow="2810" windowWidth="14400" windowHeight="7270" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Settings" sheetId="1" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="57">
   <si>
     <t>Name</t>
   </si>
@@ -166,9 +166,6 @@
     <t>OrchestratorQueueName</t>
   </si>
   <si>
-    <t>CSH-PerformerQueue</t>
-  </si>
-  <si>
     <t>QueName of the performer</t>
   </si>
   <si>
@@ -188,6 +185,15 @@
   </si>
   <si>
     <t>ACME_WorkItemsURL</t>
+  </si>
+  <si>
+    <t>MaxInitRetries</t>
+  </si>
+  <si>
+    <t>Maximum Retries for the init State on a System Exception</t>
+  </si>
+  <si>
+    <t>GYR-PerformerQueue</t>
   </si>
 </sst>
 </file>
@@ -565,8 +571,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Z998"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A13" sqref="A13"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.453125" defaultRowHeight="15" customHeight="1"/>
@@ -616,10 +622,10 @@
         <v>46</v>
       </c>
       <c r="B2" t="s">
+        <v>56</v>
+      </c>
+      <c r="C2" s="2" t="s">
         <v>47</v>
-      </c>
-      <c r="C2" s="2" t="s">
-        <v>48</v>
       </c>
       <c r="D2" s="1"/>
       <c r="E2" s="1"/>
@@ -676,6 +682,17 @@
       </c>
       <c r="C5" t="s">
         <v>45</v>
+      </c>
+    </row>
+    <row r="6" spans="1:26" ht="15" customHeight="1">
+      <c r="A6" t="s">
+        <v>54</v>
+      </c>
+      <c r="B6">
+        <v>2</v>
+      </c>
+      <c r="C6" t="s">
+        <v>55</v>
       </c>
     </row>
     <row r="7" spans="1:26" ht="14.25" customHeight="1"/>
@@ -2844,8 +2861,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:Z1000"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.453125" defaultRowHeight="15" customHeight="1"/>
@@ -2894,44 +2911,44 @@
     </row>
     <row r="2" spans="1:26" ht="14.25" customHeight="1">
       <c r="A2" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B2" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C2" t="s">
         <v>41</v>
       </c>
       <c r="D2" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="3" spans="1:26" ht="14.25" customHeight="1">
       <c r="A3" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B3" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C3" t="s">
         <v>41</v>
       </c>
       <c r="D3" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="4" spans="1:26" ht="14.25" customHeight="1">
       <c r="A4" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B4" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C4" t="s">
         <v>41</v>
       </c>
       <c r="D4" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="5" spans="1:26" ht="14.25" customHeight="1"/>

</xml_diff>